<commit_message>
added mikrobiološke to excell
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,12 +14,198 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
-  <si>
-    <t>Reaction Time</t>
-  </si>
-  <si>
-    <t>Stimulus Time</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+  <si>
+    <t>Naziv</t>
+  </si>
+  <si>
+    <t>Skupina</t>
+  </si>
+  <si>
+    <t>Opis</t>
+  </si>
+  <si>
+    <t>Sestavine</t>
+  </si>
+  <si>
+    <t>Izgled</t>
+  </si>
+  <si>
+    <t>Okus In Vonj</t>
+  </si>
+  <si>
+    <t>Zakonodaja</t>
+  </si>
+  <si>
+    <t>Salmonella</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Bacillus cereus</t>
+  </si>
+  <si>
+    <t>Skupno število</t>
+  </si>
+  <si>
+    <t>Plesni in kvasovke</t>
+  </si>
+  <si>
+    <t>Sulfitreducirajoči klostridiji</t>
+  </si>
+  <si>
+    <t>Koagulaza pozitivni stafilokoki in Staphylococcus aureus</t>
+  </si>
+  <si>
+    <t>Kvasovke in plesni</t>
+  </si>
+  <si>
+    <t>Enterobakterije</t>
+  </si>
+  <si>
+    <t>GUARANA NATURAL ENERGY 5 X 9 ml</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Naravni kofein iz gvarane in niacin v raztopini</t>
+  </si>
+  <si>
+    <t>Voda, trsni sladkor, 10 % izvleček iz semen gvarane v prahu (Paulina cupana), zgoščeni sok aronije, zgoščeni sok borovnice, uprašeni sok acerole (Malpighia glabra), niacin in konzervans: kalijev sorbat.</t>
+  </si>
+  <si>
+    <t>Temno vijolična tekočina z usedlino na dnu fiole, brez tujih primesi</t>
+  </si>
+  <si>
+    <t>Grenko sladkega okusa, aroma po borovnici in gvarani</t>
+  </si>
+  <si>
+    <t>Izdelek je v skladu z veljavno evropsko in nacionalno zakonodajo. Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP.</t>
+  </si>
+  <si>
+    <t>neg./25 g</t>
+  </si>
+  <si>
+    <t>&lt;10 CFU/g</t>
+  </si>
+  <si>
+    <t>&lt;1.000 CFU/ g</t>
+  </si>
+  <si>
+    <t>&lt;500 CFU/g</t>
+  </si>
+  <si>
+    <t>SIRUP SMREKOVI VRŠIČKI 200 ML</t>
+  </si>
+  <si>
+    <t>Sirup s smrekovimi vršički, medom in vitaminoma A in C</t>
+  </si>
+  <si>
+    <t>Med, hruškov zgoščeni sok, tekoči izvleček smrekovih vršičkov (Picea abies), tekoči izvleček listov timijana v prahu (Thymus vulgaris), tekoči izvleček listov poprove mete (Mentha x piperita), vitamin C (L-askorbinska kislina), vitamin A (retinil palmitat), olje listov evkaliptusa (Eucalyptus globulus)</t>
+  </si>
+  <si>
+    <t>svetlo rjava, viskozna tekočina</t>
+  </si>
+  <si>
+    <t>sladkega okusa, aroma po medu, timijanu, poprovi meti in evkaliptusu</t>
+  </si>
+  <si>
+    <t>neg./0,01 g</t>
+  </si>
+  <si>
+    <t>&lt; 100/g</t>
+  </si>
+  <si>
+    <t>neg./0,1 g</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>CVETNI PRAH V VREČKI 150 g</t>
+  </si>
+  <si>
+    <t>Naravni čebelji pridelek</t>
+  </si>
+  <si>
+    <t>Cvetni prah 100 %</t>
+  </si>
+  <si>
+    <t>Granule različne barve od rumene, rdeče, rjave do sive, različnih oblik in velikosti</t>
+  </si>
+  <si>
+    <t>Grenko sladkega okusa</t>
+  </si>
+  <si>
+    <t>Izdelek je v skladu z nacionalno in evropsko zakonodajo Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP</t>
+  </si>
+  <si>
+    <t>&lt; 10.000/g</t>
+  </si>
+  <si>
+    <t>MED AKACIJEV S TARTUFI 250 G</t>
+  </si>
+  <si>
+    <t>Akacijev med s tartufi</t>
+  </si>
+  <si>
+    <t>Akacijev med 99 %, črni tartufi (Tuber aestivum) 1 %</t>
+  </si>
+  <si>
+    <t>Gosta, viskozna tekočina rumene barve, z rjavimi, črnimi koščki tartufov na vrhu kozarca</t>
+  </si>
+  <si>
+    <t>Prevladujoča, značilna za tartufe</t>
+  </si>
+  <si>
+    <t>Izdelek je v skladu z veljavno nacionalno in evropsko zakonodajo. Izdelek je kontroliran v skladu s planom kontrole sistema kakovosti ISO 9001:2008, IFS in HACCP</t>
+  </si>
+  <si>
+    <t>BIO keksi pomaranča 150 g</t>
+  </si>
+  <si>
+    <t>Polnozrnati keksi s pomarančo. Slajeni z jabolčnim sokom.</t>
+  </si>
+  <si>
+    <t>Sestavine: polnozrnata pšenična moka* 61 %, rastlinska maščoba* (sončnična*, kakavova*), zgoščeni jabolčni sok* (14 %), kandirana pomarančna lupina*( 7 %), pšenični sirup* 5 %, sredstvo za vzhajanje (natrijevi karbonati). Lahko vsebuje sledove jajc, mleka, soje, volčjega boba in oreščkov. *Ekološko pridelano.</t>
+  </si>
+  <si>
+    <t>Polnozrnati keksi z odtisnjenim žitom s koščki pomarančne lupine</t>
+  </si>
+  <si>
+    <t>Žit s okusom kandirane lupine pomaranče, slajenih z jabolčnim sokom</t>
+  </si>
+  <si>
+    <t>KOLAGENBODY 150 G</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance® z magnezijem in vitaminom C v prahu</t>
+  </si>
+  <si>
+    <t>Hidrolizirani kolagen Bodybalance®, magnezijev citrat, inulin, naravni aromi, vitamin C.</t>
+  </si>
+  <si>
+    <t>Bel prah/granule</t>
+  </si>
+  <si>
+    <t>Rahlo sladkast okus po beljakovinah z aromo po citrusih</t>
+  </si>
+  <si>
+    <t>neg./1 g</t>
+  </si>
+  <si>
+    <t>&lt; 1000 cfu/g</t>
+  </si>
+  <si>
+    <t>&lt; 10 cfu/g</t>
+  </si>
+  <si>
+    <t>&lt; 100 cfu/g</t>
   </si>
 </sst>
 </file>
@@ -368,7 +554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -376,140 +562,346 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s"/>
+      <c r="O2" t="s"/>
+      <c r="P2" t="s"/>
+      <c r="Q2" t="s"/>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s"/>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" t="s"/>
+      <c r="P3" t="s"/>
+      <c r="Q3" t="s"/>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s"/>
+      <c r="I4" t="s"/>
+      <c r="J4" t="s"/>
+      <c r="K4" t="s"/>
+      <c r="L4" t="s"/>
+      <c r="M4" t="s"/>
+      <c r="N4" t="s"/>
+      <c r="O4" t="s"/>
+      <c r="P4" t="s"/>
+      <c r="Q4" t="s"/>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s"/>
+      <c r="K5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" t="s"/>
+      <c r="M5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" t="s"/>
+      <c r="Q5" t="s"/>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s"/>
+      <c r="M6" t="s"/>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" t="s"/>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s"/>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="n">
-        <v>2</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s"/>
+      <c r="I7" t="s"/>
+      <c r="J7" t="s"/>
+      <c r="K7" t="s"/>
+      <c r="L7" t="s"/>
+      <c r="M7" t="s"/>
+      <c r="N7" t="s"/>
+      <c r="O7" t="s"/>
+      <c r="P7" t="s"/>
+      <c r="Q7" t="s"/>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="n">
-        <v>4</v>
-      </c>
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B12" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="n">
-        <v>4</v>
-      </c>
-      <c r="B13" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="n">
-        <v>2</v>
-      </c>
-      <c r="B15" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="n">
-        <v>4</v>
-      </c>
-      <c r="B17" t="n">
-        <v>4</v>
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s"/>
+      <c r="J8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" t="s"/>
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+      <c r="M8" t="s"/>
+      <c r="N8" t="s">
+        <v>62</v>
+      </c>
+      <c r="O8" t="s"/>
+      <c r="P8" t="s"/>
+      <c r="Q8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>